<commit_message>
4 Şubat testleri eklenmiş excel dosyası eklendi.
</commit_message>
<xml_diff>
--- a/LOGS/Test Defteri.xlsx
+++ b/LOGS/Test Defteri.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaan Kalkandelen\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaan Kalkandelen\OneDrive\Desktop\ROKET\git\Metu-X\LOGS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBA9D0B-EF49-48E2-BF6C-A1DDDCB2A6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44C269C-3536-4998-8389-4838B7F5916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Prosedürü" sheetId="2" r:id="rId1"/>
     <sheet name="3 Şubat Testleri" sheetId="1" r:id="rId2"/>
+    <sheet name="4 Şubat Testleri" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>log0292</t>
   </si>
@@ -98,6 +99,69 @@
   </si>
   <si>
     <t xml:space="preserve">8 dereceye inme komutuna rağmen vananın kapandığını gördük. Vana tek bir derecede kapanmıyor. Vana puppettinin tam kapandığı nokta ile açık olma durumu arasında en 8 derece var. </t>
+  </si>
+  <si>
+    <t>Log alma suresi 10 saniyeden 60 saniyeye arttirildi, 90 derece 60 saniye acik kalacak sekilde ayarlandi, dry run</t>
+  </si>
+  <si>
+    <t>log0307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry runda 60snlik testi SD karta kaydetti. </t>
+  </si>
+  <si>
+    <t>log0308</t>
+  </si>
+  <si>
+    <t>Log alma suresi 10 saniyeden 60 saniyeye arttirildi, 90 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test</t>
+  </si>
+  <si>
+    <t>İlk basınçlı 60sn lik test koşuldu. 90 derecede 60sn açık kaldı sonrasında 10 dereceye düştü. Tank 50 barın altına indi. 10 derece gelirken az bir overshoot vardı. Sonrasında 10 dereceyi yakaladı. Manifoldtaki basıncın ölçümünde yine az da olsa sekmeler vardı.</t>
+  </si>
+  <si>
+    <t>log0309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180 derece 60snlik test koşuldu. Tanktaki basınç neredeyse 0 bara indi. 10 dereceye geri gelirken overshoot görüldü. </t>
+  </si>
+  <si>
+    <t>log0310</t>
+  </si>
+  <si>
+    <t>log0311</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 270 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test</t>
+  </si>
+  <si>
+    <t>180 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test</t>
+  </si>
+  <si>
+    <t>360 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">270 derece 60snlik test koşuldu. 10 dereceye inerken 5 derecenin altına düşecek şekilde overshoot görüldü. Pozisyon ve hızı yakalamada geç kaldı. Yüksek basınçta açı arttığında manifoldtaki sekmelerde artış görüldü. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">360 derece 60snlik test koşuldu.  0 a yaklaşan bir overshoot görüldü. Plakada esneme oldu. </t>
+  </si>
+  <si>
+    <t>450 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test</t>
+  </si>
+  <si>
+    <t>log0312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450 derece 60snlik test koşuldu. Açı farkı arttığından sondaki overshoot neredeyse 0 a kadar yaklaştı. Overshoottan sonra tam 10 dereceyi bulamadı. Plakada esneme görüldü. Boruların ve tüpün üstünde soğuma ve yoğuşma görüldü.  </t>
+  </si>
+  <si>
+    <t>log0313</t>
+  </si>
+  <si>
+    <t>540 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test 10 derecede overshoot 0a yaklastigi icin, sondaki vana acikligini 10 dereceden 15 dereceye cikardik.</t>
+  </si>
+  <si>
+    <t>540 derece 60snlik test koşuldu. Overshoot tekrar gözlemlendi, ama sonrasında 15 dereceyi yakaladı. Açı büyükçe başta ve sondaki current demand ve current feedback aralığı açılmaya başladı.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -568,4 +632,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2596AFA2-036F-4C42-AD93-BDA9DCDB7960}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="33.90625" customWidth="1"/>
+    <col min="3" max="3" width="31.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Post processte 12 logun 3D plot edilmesi ve bulduğumuz fonksiyonun surface olarak plotu eklendi. Hesaplamalarda baştan ve sondan 0.7 ve plotlarda baştan ve sondan 1.1 inci saniyeleri kesip işlem yapacak şekilde Mp_Np_calculation (Fonksiyon çıkarmak için) dosyası ve post process dosyası tekrardan güncellendi.
-Dünden yarım kalan testler başarıyla koşuldu ve tamamlandı.

-Excel dosyası güncellendi.
</commit_message>
<xml_diff>
--- a/LOGS/Test Defteri.xlsx
+++ b/LOGS/Test Defteri.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaan Kalkandelen\OneDrive\Desktop\ROKET\git\Metu-X\LOGS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44C269C-3536-4998-8389-4838B7F5916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB9AFC6-9539-4FFC-B7F6-0D3F6CD3DFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Prosedürü" sheetId="2" r:id="rId1"/>
     <sheet name="3 Şubat Testleri" sheetId="1" r:id="rId2"/>
     <sheet name="4 Şubat Testleri" sheetId="3" r:id="rId3"/>
+    <sheet name="5 Şubat Testleri" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>log0292</t>
   </si>
@@ -162,6 +163,60 @@
   </si>
   <si>
     <t>540 derece 60snlik test koşuldu. Overshoot tekrar gözlemlendi, ama sonrasında 15 dereceyi yakaladı. Açı büyükçe başta ve sondaki current demand ve current feedback aralığı açılmaya başladı.</t>
+  </si>
+  <si>
+    <t>log0314</t>
+  </si>
+  <si>
+    <t>630 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test.</t>
+  </si>
+  <si>
+    <t>Mustafa'nın son güncellemesi olmadan koşuldu. Dünki deneylerden farklı bir şey olmadı.</t>
+  </si>
+  <si>
+    <t>log0315</t>
+  </si>
+  <si>
+    <t>720 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mustafa'nın değişiklikleri güncellendi. Pozisyon ve hız takibi büyük oranda iyileşti. Pozisyon yakaladığı anda hız demandi ve hız feedbacki arasında fark oluyor. Özellikle Hızın yönün değişeceği durumlarda.  </t>
+  </si>
+  <si>
+    <t>810 derece 60 saniye acik kalacak sekilde ayarlandisondaki overshootun fazla olabilme ihtimali icin en son aci 20 olacak sekilde guncellendi, dolu test</t>
+  </si>
+  <si>
+    <t>log0316</t>
+  </si>
+  <si>
+    <t>Pozisyon takibi yakalandığında hız takibi yapmıyor. Gereken şekilde davranıyor. Pozisyon takibi de dünki deneylere göre daha iyi.</t>
+  </si>
+  <si>
+    <t>log0317</t>
+  </si>
+  <si>
+    <t>900 derece 60 saniye acik kalacak sekilde ayarlandisondaki overshootun fazla olabilme ihtimali icin en son aci 20 olacak sekilde guncellendi, dolu test</t>
+  </si>
+  <si>
+    <t>DeltaP oldukça azaldı birbirine yaklaşan curvelere görünüyor. Muhtemelen velocity demandi olması gerektiği gibi çalışmıyor. Pozisyon takibi oturduktan sonra hala velocity komudu vermeye devam ediyor. Vananın üstünde çok az derecede karlanma görüldü.</t>
+  </si>
+  <si>
+    <t>log0318</t>
+  </si>
+  <si>
+    <t>990 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vana 990 dereceye gelmeye çalışırken pozisyonu tam yakalayamadı. Hız takibi iyiydi. Sonda overshoot görüldü. </t>
+  </si>
+  <si>
+    <t>log0319</t>
+  </si>
+  <si>
+    <t>1080 derece 60 saniye acik kalacak sekilde ayarlandi, dolu test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vana pozisyonu önceki teste göre daha rahat yakaladı. Pozisyonda anlık titremeler görüldü. Vana üstünde yoğuşma görüldü. </t>
   </si>
 </sst>
 </file>
@@ -638,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2596AFA2-036F-4C42-AD93-BDA9DCDB7960}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -728,4 +783,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC92847C-05C6-4F47-A2F4-1A4F1F719C2E}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="25.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-- 7 Subat Yeni testlerin aciklamalari girildi
</commit_message>
<xml_diff>
--- a/LOGS/Test Defteri.xlsx
+++ b/LOGS/Test Defteri.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaan Kalkandelen\OneDrive\Desktop\ROKET\git\Metu-X\LOGS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egeel\Desktop\metux-son\Metu-X\LOGS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB9AFC6-9539-4FFC-B7F6-0D3F6CD3DFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D219517-8AF1-4E18-A4D0-DD432D7609BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Prosedürü" sheetId="2" r:id="rId1"/>
     <sheet name="3 Şubat Testleri" sheetId="1" r:id="rId2"/>
     <sheet name="4 Şubat Testleri" sheetId="3" r:id="rId3"/>
     <sheet name="5 Şubat Testleri" sheetId="4" r:id="rId4"/>
+    <sheet name="7 Subat Testleri" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
   <si>
     <t>log0292</t>
   </si>
@@ -217,6 +218,75 @@
   </si>
   <si>
     <t xml:space="preserve">Vana pozisyonu önceki teste göre daha rahat yakaladı. Pozisyonda anlık titremeler görüldü. Vana üstünde yoğuşma görüldü. </t>
+  </si>
+  <si>
+    <t>log0323</t>
+  </si>
+  <si>
+    <t>1200-30 arasi git gelli 1 snlik periyotlu basincli test, dry run</t>
+  </si>
+  <si>
+    <t>Motor istedigimiz periyodik hareketleri yapti, pozisyon ve hiz takibi beklendigi gibiydi. Dolu teste hazir</t>
+  </si>
+  <si>
+    <t>log0325</t>
+  </si>
+  <si>
+    <t>1200-30 arasi git gelli 1 snlik periyotlu basincli test</t>
+  </si>
+  <si>
+    <t>Motor beklenen hareketi gerceklestirdi. 60 saniyenin sonunda 30 derece kapanma beklerken pos_feedback degeri 120 civari gosteriyordu. Ancak, biz elle kapatmayi deneyince tamamen kapaliydi, hizini alamamis olabilir mi?</t>
+  </si>
+  <si>
+    <t>600 derece ofsetli 80 derece magnitude 5Hz sinus fonksiyonudry run</t>
+  </si>
+  <si>
+    <t>log0332</t>
+  </si>
+  <si>
+    <t>Test amacli dry run kosuldu</t>
+  </si>
+  <si>
+    <t>log0335</t>
+  </si>
+  <si>
+    <t>600 derece ofsetli 80 derece magnitude 5Hz sinus fonksiyonubasincli test</t>
+  </si>
+  <si>
+    <t>Hiz 400RPMde 0.05sn kaldi tepe degeri olarak. Hiz ve pozisyon takibi iyi. Baglanti koptugundan log kaydetme ilginc bir sekilde yarida kesildi. Basinc sonda 20 bara kadar dustu. Test 17.5 sn surdu</t>
+  </si>
+  <si>
+    <t>log0339</t>
+  </si>
+  <si>
+    <t>600 derece ofsetli 40 derece magnitude 10Hz sinus fonksiyonubasincli test</t>
+  </si>
+  <si>
+    <t>Hiz 400RPMe ulasmadan azaliyor, istedigimiz gibi. Pozisyon ve hiz takibi iyi. Log basarili kaydoldu.</t>
+  </si>
+  <si>
+    <t>log0336</t>
+  </si>
+  <si>
+    <t>Dry Run</t>
+  </si>
+  <si>
+    <t>log0343</t>
+  </si>
+  <si>
+    <t>600 derece ofsetli 25 derece magnitude 15Hz sinus fonksiyonubasincli test</t>
+  </si>
+  <si>
+    <t>600 derece ofsetli 25 derece magnitude 15Hz sinus fonksiyonu dry run</t>
+  </si>
+  <si>
+    <t>Dry Run. Hiz demandi 400 olmasina ragmen motor hizi yakalayamadi. Bu testin ardindan 30 dereceli bir dry run kosuldu, onda hiz demandi 400RPM'de belli bir sure stabil kaldigindan dolayi 25 dereceye geri cektik. STLink baglanti kopmasaini onlemek icin USB soketinin ustune cift tarafli bant yapistirdik, titresimden dolayi baglanti kopuyordu.</t>
+  </si>
+  <si>
+    <t>log0345</t>
+  </si>
+  <si>
+    <t>Hiz demandini yakalayamadigi icin pozisyon takibi neredeyse 1 faz kadar gecikti. Sinus neredeyse cosinus'e donustu. Baglanti cift tarafli bant sayesinde kopmadi.</t>
   </si>
 </sst>
 </file>
@@ -252,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -262,6 +332,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC92847C-05C6-4F47-A2F4-1A4F1F719C2E}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,4 +947,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A6DA89C-2906-41F5-95CA-635D68041747}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.36328125" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="116" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>